<commit_message>
Exercise 16. Get contacts and groups lists from data base. Verification UI and data base information
</commit_message>
<xml_diff>
--- a/solution_adressbook_tests/adressbook_tests/groups.xlsx
+++ b/solution_adressbook_tests/adressbook_tests/groups.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>w</t>
   </si>
@@ -25,75 +25,6 @@
   </si>
   <si>
     <t>xkarqak</t>
-  </si>
-  <si>
-    <t>sihlhc</t>
-  </si>
-  <si>
-    <t>qab</t>
-  </si>
-  <si>
-    <t>olnewbk</t>
-  </si>
-  <si>
-    <t>fustf</t>
-  </si>
-  <si>
-    <t>txogj</t>
-  </si>
-  <si>
-    <t>lsgsym</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>lwcqdmwu</t>
-  </si>
-  <si>
-    <t>ooxkxong</t>
-  </si>
-  <si>
-    <t>ibskpjg</t>
-  </si>
-  <si>
-    <t>fufjbiki</t>
-  </si>
-  <si>
-    <t>vqo</t>
-  </si>
-  <si>
-    <t>hbsk</t>
-  </si>
-  <si>
-    <t>bniidlg</t>
-  </si>
-  <si>
-    <t>ta</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>rj</t>
-  </si>
-  <si>
-    <t>gcp</t>
-  </si>
-  <si>
-    <t>ngmb</t>
-  </si>
-  <si>
-    <t>rvqia</t>
-  </si>
-  <si>
-    <t>yuismwrsc</t>
-  </si>
-  <si>
-    <t>njfipxec</t>
-  </si>
-  <si>
-    <t>dyguagtko</t>
   </si>
 </sst>
 </file>
@@ -433,11 +364,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -452,93 +381,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>